<commit_message>
Added level 5 + starting player location
</commit_message>
<xml_diff>
--- a/Assets/Level_Tool.xlsx
+++ b/Assets/Level_Tool.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scote/Desktop/DOSSIER PERSO/ArduBoy Projects files/SpaceCab/Assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scote/Downloads/SpaceCab-master/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C672B682-D2D7-3642-BB3F-3DD6C30B71CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{856ABBDD-7C0B-9742-A95A-8A5190B31794}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71200" yWindow="1400" windowWidth="28040" windowHeight="26880" xr2:uid="{034143F2-81DD-E240-A4FE-E146F63DCD7B}"/>
+    <workbookView xWindow="62400" yWindow="460" windowWidth="28040" windowHeight="26880" xr2:uid="{034143F2-81DD-E240-A4FE-E146F63DCD7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="22">
   <si>
     <t xml:space="preserve">PLAT1, </t>
   </si>
@@ -89,6 +89,12 @@
   <si>
     <t>SPIKD,</t>
   </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>PLAYER SPAWN</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +122,7 @@
       <name val="Calibri (Corps)_x0000_"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +219,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC990FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -226,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -245,12 +257,18 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC990FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -562,10 +580,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ121"/>
+  <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="W76" sqref="W76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1104,9 +1122,7 @@
       <c r="T7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U7" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="U7" s="18"/>
       <c r="V7" s="6" t="s">
         <v>8</v>
       </c>
@@ -2113,7 +2129,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="16" customHeight="1">
+    <row r="17" spans="1:37" ht="16" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -2220,7 +2236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="16" customHeight="1">
+    <row r="18" spans="1:37" ht="16" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -2327,7 +2343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:37">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -2363,7 +2379,7 @@
       <c r="AG19" s="17"/>
       <c r="AH19" s="17"/>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:37">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -2399,12 +2415,16 @@
       <c r="AG20" s="17"/>
       <c r="AH20" s="17"/>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:37">
       <c r="A21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:36">
+      <c r="AJ21" s="18"/>
+      <c r="AK21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2508,7 +2528,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:37">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2544,7 +2564,7 @@
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:37">
       <c r="A24" s="14" t="s">
         <v>14</v>
       </c>
@@ -2648,7 +2668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:37">
       <c r="A25" s="4" t="s">
         <v>1</v>
       </c>
@@ -2752,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:37">
       <c r="A26" s="4" t="s">
         <v>1</v>
       </c>
@@ -2856,7 +2876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:37">
       <c r="A27" s="4" t="s">
         <v>1</v>
       </c>
@@ -2960,7 +2980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:37">
       <c r="A28" s="4" t="s">
         <v>1</v>
       </c>
@@ -3064,7 +3084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:37">
       <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
@@ -3168,7 +3188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:37">
       <c r="A30" s="4" t="s">
         <v>1</v>
       </c>
@@ -3272,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:37">
       <c r="A31" s="12" t="s">
         <v>17</v>
       </c>
@@ -3376,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:37">
       <c r="A32" s="12" t="s">
         <v>17</v>
       </c>
@@ -3930,9 +3950,7 @@
       <c r="K37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L37" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="L37" s="18"/>
       <c r="M37" s="6" t="s">
         <v>8</v>
       </c>
@@ -5535,9 +5553,7 @@
       <c r="W55" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="X55" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="X55" s="18"/>
       <c r="Y55" s="8" t="s">
         <v>2</v>
       </c>
@@ -6310,20 +6326,20 @@
       <c r="A66" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>1</v>
+      <c r="B66" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>1</v>
+      <c r="D66" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>1</v>
@@ -6732,8 +6748,8 @@
       <c r="C70" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>1</v>
+      <c r="D70" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>1</v>
@@ -6839,8 +6855,8 @@
       <c r="D71" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>1</v>
+      <c r="E71" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>1</v>
@@ -6946,8 +6962,8 @@
       <c r="E72" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>1</v>
+      <c r="F72" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>1</v>
@@ -7053,32 +7069,30 @@
       <c r="F73" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>1</v>
+      <c r="G73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I73" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="J73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N73" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O73" s="4" t="s">
-        <v>1</v>
+      <c r="K73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M73" s="18"/>
+      <c r="N73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O73" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="P73" s="4" t="s">
         <v>1</v>
@@ -7731,652 +7745,1707 @@
       <c r="AH80" s="17"/>
     </row>
     <row r="81" spans="1:34">
-      <c r="A81" s="17"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="17"/>
-      <c r="L81" s="17"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="17"/>
-      <c r="R81" s="17"/>
-      <c r="S81" s="17"/>
-      <c r="T81" s="17"/>
-      <c r="U81" s="17"/>
-      <c r="V81" s="17"/>
-      <c r="W81" s="17"/>
-      <c r="X81" s="17"/>
-      <c r="Y81" s="17"/>
-      <c r="Z81" s="17"/>
-      <c r="AA81" s="17"/>
-      <c r="AB81" s="17"/>
-      <c r="AC81" s="17"/>
-      <c r="AD81" s="17"/>
-      <c r="AE81" s="17"/>
-      <c r="AF81" s="17"/>
-      <c r="AG81" s="17"/>
-      <c r="AH81" s="17"/>
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="82" spans="1:34">
-      <c r="A82" s="17"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="17"/>
-      <c r="K82" s="17"/>
-      <c r="L82" s="17"/>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
-      <c r="P82" s="17"/>
-      <c r="Q82" s="17"/>
-      <c r="R82" s="17"/>
-      <c r="S82" s="17"/>
-      <c r="T82" s="17"/>
-      <c r="U82" s="17"/>
-      <c r="V82" s="17"/>
-      <c r="W82" s="17"/>
-      <c r="X82" s="17"/>
-      <c r="Y82" s="17"/>
-      <c r="Z82" s="17"/>
-      <c r="AA82" s="17"/>
-      <c r="AB82" s="17"/>
-      <c r="AC82" s="17"/>
-      <c r="AD82" s="17"/>
-      <c r="AE82" s="17"/>
-      <c r="AF82" s="17"/>
-      <c r="AG82" s="17"/>
-      <c r="AH82" s="17"/>
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82">
+        <v>6</v>
+      </c>
+      <c r="H82">
+        <v>7</v>
+      </c>
+      <c r="I82">
+        <v>8</v>
+      </c>
+      <c r="J82">
+        <v>9</v>
+      </c>
+      <c r="K82">
+        <v>10</v>
+      </c>
+      <c r="L82">
+        <v>11</v>
+      </c>
+      <c r="M82">
+        <v>12</v>
+      </c>
+      <c r="N82">
+        <v>13</v>
+      </c>
+      <c r="O82">
+        <v>14</v>
+      </c>
+      <c r="P82">
+        <v>15</v>
+      </c>
+      <c r="Q82">
+        <v>16</v>
+      </c>
+      <c r="R82">
+        <v>17</v>
+      </c>
+      <c r="S82">
+        <v>18</v>
+      </c>
+      <c r="T82">
+        <v>19</v>
+      </c>
+      <c r="U82">
+        <v>20</v>
+      </c>
+      <c r="V82">
+        <v>21</v>
+      </c>
+      <c r="W82">
+        <v>22</v>
+      </c>
+      <c r="X82">
+        <v>23</v>
+      </c>
+      <c r="Y82">
+        <v>24</v>
+      </c>
+      <c r="Z82">
+        <v>25</v>
+      </c>
+      <c r="AA82">
+        <v>26</v>
+      </c>
+      <c r="AB82">
+        <v>27</v>
+      </c>
+      <c r="AC82">
+        <v>28</v>
+      </c>
+      <c r="AD82">
+        <v>29</v>
+      </c>
+      <c r="AE82">
+        <v>30</v>
+      </c>
+      <c r="AF82">
+        <v>31</v>
+      </c>
+      <c r="AG82">
+        <v>32</v>
+      </c>
+      <c r="AH82">
+        <v>33</v>
+      </c>
     </row>
     <row r="83" spans="1:34">
-      <c r="A83" s="17"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17"/>
-      <c r="K83" s="17"/>
-      <c r="L83" s="17"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
-      <c r="Q83" s="17"/>
-      <c r="R83" s="17"/>
-      <c r="S83" s="17"/>
-      <c r="T83" s="17"/>
-      <c r="U83" s="17"/>
-      <c r="V83" s="17"/>
-      <c r="W83" s="17"/>
-      <c r="X83" s="17"/>
-      <c r="Y83" s="17"/>
-      <c r="Z83" s="17"/>
-      <c r="AA83" s="17"/>
-      <c r="AB83" s="17"/>
-      <c r="AC83" s="17"/>
-      <c r="AD83" s="17"/>
-      <c r="AE83" s="17"/>
-      <c r="AF83" s="17"/>
-      <c r="AG83" s="17"/>
-      <c r="AH83" s="17"/>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+      <c r="Y83" s="1"/>
+      <c r="Z83" s="1"/>
+      <c r="AA83" s="1"/>
+      <c r="AB83" s="1"/>
+      <c r="AC83" s="1"/>
+      <c r="AD83" s="1"/>
+      <c r="AE83" s="1"/>
+      <c r="AF83" s="1"/>
+      <c r="AG83" s="1"/>
+      <c r="AH83" s="1"/>
     </row>
     <row r="84" spans="1:34">
-      <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="17"/>
-      <c r="L84" s="17"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
-      <c r="Q84" s="17"/>
-      <c r="R84" s="17"/>
-      <c r="S84" s="17"/>
-      <c r="T84" s="17"/>
-      <c r="U84" s="17"/>
-      <c r="V84" s="17"/>
-      <c r="W84" s="17"/>
-      <c r="X84" s="17"/>
-      <c r="Y84" s="17"/>
-      <c r="Z84" s="17"/>
-      <c r="AA84" s="17"/>
-      <c r="AB84" s="17"/>
-      <c r="AC84" s="17"/>
-      <c r="AD84" s="17"/>
-      <c r="AE84" s="17"/>
-      <c r="AF84" s="17"/>
-      <c r="AG84" s="17"/>
-      <c r="AH84" s="17"/>
+      <c r="A84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P84" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q84" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="R84" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="S84" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="T84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH84" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="85" spans="1:34">
-      <c r="A85" s="17"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="17"/>
-      <c r="L85" s="17"/>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17"/>
-      <c r="Q85" s="17"/>
-      <c r="R85" s="17"/>
-      <c r="S85" s="17"/>
-      <c r="T85" s="17"/>
-      <c r="U85" s="17"/>
-      <c r="V85" s="17"/>
-      <c r="W85" s="17"/>
-      <c r="X85" s="17"/>
-      <c r="Y85" s="17"/>
-      <c r="Z85" s="17"/>
-      <c r="AA85" s="17"/>
-      <c r="AB85" s="17"/>
-      <c r="AC85" s="17"/>
-      <c r="AD85" s="17"/>
-      <c r="AE85" s="17"/>
-      <c r="AF85" s="17"/>
-      <c r="AG85" s="17"/>
-      <c r="AH85" s="17"/>
+      <c r="A85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="V85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="W85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="X85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG85" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH85" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="86" spans="1:34">
-      <c r="A86" s="17"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="17"/>
-      <c r="L86" s="17"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="17"/>
-      <c r="R86" s="17"/>
-      <c r="S86" s="17"/>
-      <c r="T86" s="17"/>
-      <c r="U86" s="17"/>
-      <c r="V86" s="17"/>
-      <c r="W86" s="17"/>
-      <c r="X86" s="17"/>
-      <c r="Y86" s="17"/>
-      <c r="Z86" s="17"/>
-      <c r="AA86" s="17"/>
-      <c r="AB86" s="17"/>
-      <c r="AC86" s="17"/>
-      <c r="AD86" s="17"/>
-      <c r="AE86" s="17"/>
-      <c r="AF86" s="17"/>
-      <c r="AG86" s="17"/>
-      <c r="AH86" s="17"/>
+      <c r="A86" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K86" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O86" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T86" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="U86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE86" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF86" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG86" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH86" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="87" spans="1:34">
-      <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="17"/>
-      <c r="L87" s="17"/>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
-      <c r="P87" s="17"/>
-      <c r="Q87" s="17"/>
-      <c r="R87" s="17"/>
-      <c r="S87" s="17"/>
-      <c r="T87" s="17"/>
-      <c r="U87" s="17"/>
-      <c r="V87" s="17"/>
-      <c r="W87" s="17"/>
-      <c r="X87" s="17"/>
-      <c r="Y87" s="17"/>
-      <c r="Z87" s="17"/>
-      <c r="AA87" s="17"/>
-      <c r="AB87" s="17"/>
-      <c r="AC87" s="17"/>
-      <c r="AD87" s="17"/>
-      <c r="AE87" s="17"/>
-      <c r="AF87" s="17"/>
-      <c r="AG87" s="17"/>
-      <c r="AH87" s="17"/>
+      <c r="A87" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="18"/>
+      <c r="F87" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K87" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF87" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG87" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH87" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="88" spans="1:34">
-      <c r="A88" s="17"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="17"/>
-      <c r="K88" s="17"/>
-      <c r="L88" s="17"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
-      <c r="Q88" s="17"/>
-      <c r="R88" s="17"/>
-      <c r="S88" s="17"/>
-      <c r="T88" s="17"/>
-      <c r="U88" s="17"/>
-      <c r="V88" s="17"/>
-      <c r="W88" s="17"/>
-      <c r="X88" s="17"/>
-      <c r="Y88" s="17"/>
-      <c r="Z88" s="17"/>
-      <c r="AA88" s="17"/>
-      <c r="AB88" s="17"/>
-      <c r="AC88" s="17"/>
-      <c r="AD88" s="17"/>
-      <c r="AE88" s="17"/>
-      <c r="AF88" s="17"/>
-      <c r="AG88" s="17"/>
-      <c r="AH88" s="17"/>
+      <c r="A88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE88" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH88" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="89" spans="1:34">
-      <c r="A89" s="17"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="17"/>
-      <c r="L89" s="17"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="17"/>
-      <c r="P89" s="17"/>
-      <c r="Q89" s="17"/>
-      <c r="R89" s="17"/>
-      <c r="S89" s="17"/>
-      <c r="T89" s="17"/>
-      <c r="U89" s="17"/>
-      <c r="V89" s="17"/>
-      <c r="W89" s="17"/>
-      <c r="X89" s="17"/>
-      <c r="Y89" s="17"/>
-      <c r="Z89" s="17"/>
-      <c r="AA89" s="17"/>
-      <c r="AB89" s="17"/>
-      <c r="AC89" s="17"/>
-      <c r="AD89" s="17"/>
-      <c r="AE89" s="17"/>
-      <c r="AF89" s="17"/>
-      <c r="AG89" s="17"/>
-      <c r="AH89" s="17"/>
+      <c r="A89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG89" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH89" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="90" spans="1:34">
-      <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
-      <c r="Q90" s="17"/>
-      <c r="R90" s="17"/>
-      <c r="S90" s="17"/>
-      <c r="T90" s="17"/>
-      <c r="U90" s="17"/>
-      <c r="V90" s="17"/>
-      <c r="W90" s="17"/>
-      <c r="X90" s="17"/>
-      <c r="Y90" s="17"/>
-      <c r="Z90" s="17"/>
-      <c r="AA90" s="17"/>
-      <c r="AB90" s="17"/>
-      <c r="AC90" s="17"/>
-      <c r="AD90" s="17"/>
-      <c r="AE90" s="17"/>
-      <c r="AF90" s="17"/>
-      <c r="AG90" s="17"/>
-      <c r="AH90" s="17"/>
+      <c r="A90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="S90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U90" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH90" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="91" spans="1:34">
-      <c r="A91" s="17"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="17"/>
-      <c r="L91" s="17"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="17"/>
-      <c r="R91" s="17"/>
-      <c r="S91" s="17"/>
-      <c r="T91" s="17"/>
-      <c r="U91" s="17"/>
-      <c r="V91" s="17"/>
-      <c r="W91" s="17"/>
-      <c r="X91" s="17"/>
-      <c r="Y91" s="17"/>
-      <c r="Z91" s="17"/>
-      <c r="AA91" s="17"/>
-      <c r="AB91" s="17"/>
-      <c r="AC91" s="17"/>
-      <c r="AD91" s="17"/>
-      <c r="AE91" s="17"/>
-      <c r="AF91" s="17"/>
-      <c r="AG91" s="17"/>
-      <c r="AH91" s="17"/>
+      <c r="A91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="S91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="T91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG91" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH91" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="92" spans="1:34">
-      <c r="A92" s="17"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="17"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92" s="17"/>
-      <c r="J92" s="17"/>
-      <c r="K92" s="17"/>
-      <c r="L92" s="17"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="17"/>
-      <c r="Q92" s="17"/>
-      <c r="R92" s="17"/>
-      <c r="S92" s="17"/>
-      <c r="T92" s="17"/>
-      <c r="U92" s="17"/>
-      <c r="V92" s="17"/>
-      <c r="W92" s="17"/>
-      <c r="X92" s="17"/>
-      <c r="Y92" s="17"/>
-      <c r="Z92" s="17"/>
-      <c r="AA92" s="17"/>
-      <c r="AB92" s="17"/>
-      <c r="AC92" s="17"/>
-      <c r="AD92" s="17"/>
-      <c r="AE92" s="17"/>
-      <c r="AF92" s="17"/>
-      <c r="AG92" s="17"/>
-      <c r="AH92" s="17"/>
+      <c r="A92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="R92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="S92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="T92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="U92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH92" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="93" spans="1:34">
-      <c r="A93" s="17"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="17"/>
-      <c r="L93" s="17"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="17"/>
-      <c r="Q93" s="17"/>
-      <c r="R93" s="17"/>
-      <c r="S93" s="17"/>
-      <c r="T93" s="17"/>
-      <c r="U93" s="17"/>
-      <c r="V93" s="17"/>
-      <c r="W93" s="17"/>
-      <c r="X93" s="17"/>
-      <c r="Y93" s="17"/>
-      <c r="Z93" s="17"/>
-      <c r="AA93" s="17"/>
-      <c r="AB93" s="17"/>
-      <c r="AC93" s="17"/>
-      <c r="AD93" s="17"/>
-      <c r="AE93" s="17"/>
-      <c r="AF93" s="17"/>
-      <c r="AG93" s="17"/>
-      <c r="AH93" s="17"/>
+      <c r="A93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG93" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH93" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="94" spans="1:34">
-      <c r="A94" s="17"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="17"/>
-      <c r="J94" s="17"/>
-      <c r="K94" s="17"/>
-      <c r="L94" s="17"/>
-      <c r="M94" s="17"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="17"/>
-      <c r="Q94" s="17"/>
-      <c r="R94" s="17"/>
-      <c r="S94" s="17"/>
-      <c r="T94" s="17"/>
-      <c r="U94" s="17"/>
-      <c r="V94" s="17"/>
-      <c r="W94" s="17"/>
-      <c r="X94" s="17"/>
-      <c r="Y94" s="17"/>
-      <c r="Z94" s="17"/>
-      <c r="AA94" s="17"/>
-      <c r="AB94" s="17"/>
-      <c r="AC94" s="17"/>
-      <c r="AD94" s="17"/>
-      <c r="AE94" s="17"/>
-      <c r="AF94" s="17"/>
-      <c r="AG94" s="17"/>
-      <c r="AH94" s="17"/>
+      <c r="A94" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF94" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG94" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH94" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="95" spans="1:34">
-      <c r="A95" s="17"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="17"/>
-      <c r="L95" s="17"/>
-      <c r="M95" s="17"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="17"/>
-      <c r="Q95" s="17"/>
-      <c r="R95" s="17"/>
-      <c r="S95" s="17"/>
-      <c r="T95" s="17"/>
-      <c r="U95" s="17"/>
-      <c r="V95" s="17"/>
-      <c r="W95" s="17"/>
-      <c r="X95" s="17"/>
-      <c r="Y95" s="17"/>
-      <c r="Z95" s="17"/>
-      <c r="AA95" s="17"/>
-      <c r="AB95" s="17"/>
-      <c r="AC95" s="17"/>
-      <c r="AD95" s="17"/>
-      <c r="AE95" s="17"/>
-      <c r="AF95" s="17"/>
-      <c r="AG95" s="17"/>
-      <c r="AH95" s="17"/>
+      <c r="A95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P95" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH95" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="96" spans="1:34">
-      <c r="A96" s="17"/>
-      <c r="B96" s="17"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="17"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="17"/>
-      <c r="K96" s="17"/>
-      <c r="L96" s="17"/>
-      <c r="M96" s="17"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="17"/>
-      <c r="Q96" s="17"/>
-      <c r="R96" s="17"/>
-      <c r="S96" s="17"/>
-      <c r="T96" s="17"/>
-      <c r="U96" s="17"/>
-      <c r="V96" s="17"/>
-      <c r="W96" s="17"/>
-      <c r="X96" s="17"/>
-      <c r="Y96" s="17"/>
-      <c r="Z96" s="17"/>
-      <c r="AA96" s="17"/>
-      <c r="AB96" s="17"/>
-      <c r="AC96" s="17"/>
-      <c r="AD96" s="17"/>
-      <c r="AE96" s="17"/>
-      <c r="AF96" s="17"/>
-      <c r="AG96" s="17"/>
-      <c r="AH96" s="17"/>
+      <c r="A96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J96" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="S96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="T96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH96" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="97" spans="1:34">
-      <c r="A97" s="17"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="17"/>
-      <c r="J97" s="17"/>
-      <c r="K97" s="17"/>
-      <c r="L97" s="17"/>
-      <c r="M97" s="17"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="17"/>
-      <c r="Q97" s="17"/>
-      <c r="R97" s="17"/>
-      <c r="S97" s="17"/>
-      <c r="T97" s="17"/>
-      <c r="U97" s="17"/>
-      <c r="V97" s="17"/>
-      <c r="W97" s="17"/>
-      <c r="X97" s="17"/>
-      <c r="Y97" s="17"/>
-      <c r="Z97" s="17"/>
-      <c r="AA97" s="17"/>
-      <c r="AB97" s="17"/>
-      <c r="AC97" s="17"/>
-      <c r="AD97" s="17"/>
-      <c r="AE97" s="17"/>
-      <c r="AF97" s="17"/>
-      <c r="AG97" s="17"/>
-      <c r="AH97" s="17"/>
+      <c r="A97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="S97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="T97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="W97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="X97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB97" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG97" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH97" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="98" spans="1:34">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="17"/>
-      <c r="K98" s="17"/>
-      <c r="L98" s="17"/>
-      <c r="M98" s="17"/>
-      <c r="N98" s="17"/>
-      <c r="O98" s="17"/>
-      <c r="P98" s="17"/>
-      <c r="Q98" s="17"/>
-      <c r="R98" s="17"/>
-      <c r="S98" s="17"/>
-      <c r="T98" s="17"/>
-      <c r="U98" s="17"/>
-      <c r="V98" s="17"/>
-      <c r="W98" s="17"/>
-      <c r="X98" s="17"/>
-      <c r="Y98" s="17"/>
-      <c r="Z98" s="17"/>
-      <c r="AA98" s="17"/>
-      <c r="AB98" s="17"/>
-      <c r="AC98" s="17"/>
-      <c r="AD98" s="17"/>
-      <c r="AE98" s="17"/>
-      <c r="AF98" s="17"/>
-      <c r="AG98" s="17"/>
-      <c r="AH98" s="17"/>
+      <c r="A98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="S98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="T98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG98" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH98" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="99" spans="1:34">
       <c r="A99" s="17"/>

</xml_diff>